<commit_message>
Updated analysis data per log obtained
</commit_message>
<xml_diff>
--- a/analysis/New design vs Range queries Benchmark.xlsx
+++ b/analysis/New design vs Range queries Benchmark.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="18980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="18960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,6 +88,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <i/>
       <sz val="12"/>
       <color theme="1"/>
@@ -137,7 +146,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -145,6 +154,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -420,11 +430,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1423530880"/>
-        <c:axId val="-1423528560"/>
+        <c:axId val="1574028544"/>
+        <c:axId val="1574031024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1423530880"/>
+        <c:axId val="1574028544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -467,7 +477,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1423528560"/>
+        <c:crossAx val="1574031024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -475,7 +485,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1423528560"/>
+        <c:axId val="1574031024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -525,7 +535,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1423530880"/>
+        <c:crossAx val="1574028544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1449,8 +1459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="163" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A8" zoomScale="163" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1858,21 +1868,21 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C26">
@@ -1889,7 +1899,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C27">
@@ -1906,7 +1916,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C28">
@@ -1923,7 +1933,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C29">

</xml_diff>

<commit_message>
Added HyperDex instrumentation in S3 tests, updated analysis graphs with axis names.
</commit_message>
<xml_diff>
--- a/analysis/New design vs Range queries Benchmark.xlsx
+++ b/analysis/New design vs Range queries Benchmark.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="11">
   <si>
     <t>[1000]</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Averages</t>
+  </si>
+  <si>
+    <t>Labelled</t>
   </si>
 </sst>
 </file>
@@ -185,6 +188,52 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Retrieval</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> t</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>imes for</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>labelled chunks (1000)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs. range queries</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -430,11 +479,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1574028544"/>
-        <c:axId val="1574031024"/>
+        <c:axId val="-1870959552"/>
+        <c:axId val="-1870956800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1574028544"/>
+        <c:axId val="-1870959552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -477,7 +526,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1574031024"/>
+        <c:crossAx val="-1870956800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -485,7 +534,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1574031024"/>
+        <c:axId val="-1870956800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,6 +554,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time to retrieve range, ms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -535,7 +640,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1574028544"/>
+        <c:crossAx val="-1870959552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1459,8 +1564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A8" zoomScale="163" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:B29"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" zoomScale="163" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1882,6 +1987,9 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="B26" s="5" t="s">
         <v>0</v>
       </c>
@@ -1907,11 +2015,11 @@
         <v>85.523526333333336</v>
       </c>
       <c r="D27">
-        <f t="shared" ref="D27:D29" si="4">G19</f>
+        <f>G19</f>
         <v>60.418230999999999</v>
       </c>
       <c r="E27">
-        <f t="shared" ref="E27:E28" si="5">K19</f>
+        <f t="shared" ref="E27:E28" si="4">K19</f>
         <v>60.258470333333328</v>
       </c>
     </row>
@@ -1928,7 +2036,7 @@
         <v>101.76266933333333</v>
       </c>
       <c r="E28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>110.46768366666667</v>
       </c>
     </row>
@@ -1941,7 +2049,7 @@
         <v>149.21793233333332</v>
       </c>
       <c r="D29">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D27:D29" si="5">G21</f>
         <v>144.92579466666666</v>
       </c>
       <c r="E29">

</xml_diff>